<commit_message>
Fixed error in excess mortality decomposition
</commit_message>
<xml_diff>
--- a/Output/AppendixTab6.xlsx
+++ b/Output/AppendixTab6.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,156 +409,72 @@
         <v>19</v>
       </c>
       <c r="C2">
+        <v>0.03100350615901237</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>5.072292804305512e-005</v>
-      </c>
       <c r="E2">
-        <v>1.578114968057618e-006</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>4.91448130749975e-005</v>
-      </c>
-      <c r="G2">
-        <v>0.0311124579937118</v>
-      </c>
-      <c r="H2">
-        <v>0.9688875420062881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.1028601175810952</v>
       </c>
       <c r="D3">
-        <v>5.072292804305512e-005</v>
+        <v>-0.07185661142208284</v>
       </c>
       <c r="E3">
-        <v>7.006514237503778e-007</v>
+        <v>-0.03764720162676073</v>
       </c>
       <c r="F3">
-        <v>5.002227661930474e-005</v>
+        <v>-0.0342094097953221</v>
       </c>
       <c r="G3">
-        <v>0.0138133079217281</v>
+        <v>0.5239211936341194</v>
       </c>
       <c r="H3">
-        <v>0.9861866920782718</v>
+        <v>0.4760788063658806</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>5.072292804305512e-005</v>
+        <v>0.171962429438217</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-0.1409589232792046</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.06023535845635434</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>0.002238285045403239</v>
-      </c>
-      <c r="D5">
-        <v>-0.002187562117360184</v>
-      </c>
-      <c r="E5">
-        <v>-0.0005844273885279419</v>
-      </c>
-      <c r="F5">
-        <v>-0.001603134728832242</v>
-      </c>
-      <c r="G5">
-        <v>0.26715921979541</v>
-      </c>
-      <c r="H5">
-        <v>0.73284078020459</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>0.01205758472528257</v>
-      </c>
-      <c r="D6">
-        <v>-0.01200686179723952</v>
-      </c>
-      <c r="E6">
-        <v>0.001002094259834339</v>
-      </c>
-      <c r="F6">
-        <v>-0.01300895605707386</v>
-      </c>
-      <c r="G6">
-        <v>0.071521708734786</v>
-      </c>
-      <c r="H6">
-        <v>0.9284782912652141</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>0.022214568065484</v>
-      </c>
-      <c r="D7">
-        <v>-0.02216384513744095</v>
-      </c>
-      <c r="E7">
-        <v>-0.002409237225154463</v>
-      </c>
-      <c r="F7">
-        <v>-0.01975460791228649</v>
-      </c>
-      <c r="G7">
-        <v>0.1087012298729964</v>
-      </c>
-      <c r="H7">
-        <v>0.8912987701270035</v>
+        <v>-0.0807235648228503</v>
+      </c>
+      <c r="G4">
+        <v>0.427325614122655</v>
+      </c>
+      <c r="H4">
+        <v>0.5726743858773449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some errors when aggregating data
</commit_message>
<xml_diff>
--- a/Output/AppendixTab6.xlsx
+++ b/Output/AppendixTab6.xlsx
@@ -409,7 +409,7 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>0.03100350615901237</v>
+        <v>0.06653805445417677</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -431,22 +431,22 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>0.1028601175810952</v>
+        <v>0.2179061588686753</v>
       </c>
       <c r="D3">
-        <v>-0.07185661142208284</v>
+        <v>-0.1513681044144985</v>
       </c>
       <c r="E3">
-        <v>-0.03764720162676073</v>
+        <v>-0.0767665620947065</v>
       </c>
       <c r="F3">
-        <v>-0.0342094097953221</v>
+        <v>-0.07460154231979201</v>
       </c>
       <c r="G3">
-        <v>0.5239211936341194</v>
+        <v>0.5071515058713623</v>
       </c>
       <c r="H3">
-        <v>0.4760788063658806</v>
+        <v>0.4928484941286379</v>
       </c>
     </row>
     <row r="4">
@@ -459,22 +459,22 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>0.171962429438217</v>
+        <v>0.2250579911111283</v>
       </c>
       <c r="D4">
-        <v>-0.1409589232792046</v>
+        <v>-0.1585199366569516</v>
       </c>
       <c r="E4">
-        <v>-0.06023535845635434</v>
+        <v>-0.08886230598376316</v>
       </c>
       <c r="F4">
-        <v>-0.0807235648228503</v>
+        <v>-0.06965763067318842</v>
       </c>
       <c r="G4">
-        <v>0.427325614122655</v>
+        <v>0.5605749526387177</v>
       </c>
       <c r="H4">
-        <v>0.5726743858773449</v>
+        <v>0.4394250473612823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor update of results
</commit_message>
<xml_diff>
--- a/Output/AppendixTab6.xlsx
+++ b/Output/AppendixTab6.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,75 +406,187 @@
         </is>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>0.06653805445417677</v>
+        <v>0.06464924231864996</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.001925425130163749</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0004161797637778281</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.001509245366385914</v>
+      </c>
+      <c r="G2">
+        <v>0.216149543941205</v>
+      </c>
+      <c r="H2">
+        <v>0.783850456058795</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>0.2179061588686753</v>
+        <v>0.06513333139719893</v>
       </c>
       <c r="D3">
-        <v>-0.1513681044144985</v>
+        <v>0.001441336051614783</v>
       </c>
       <c r="E3">
-        <v>-0.0767665620947065</v>
+        <v>0.0001703283534777427</v>
       </c>
       <c r="F3">
-        <v>-0.07460154231979201</v>
+        <v>0.001271007698137038</v>
       </c>
       <c r="G3">
-        <v>0.5071515058713623</v>
+        <v>0.1181739354170165</v>
       </c>
       <c r="H3">
-        <v>0.4928484941286379</v>
+        <v>0.8818260645829835</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>0.06532623255231347</v>
+      </c>
+      <c r="D4">
+        <v>0.001248434896500242</v>
+      </c>
+      <c r="E4">
+        <v>6.138049671319686e-005</v>
+      </c>
+      <c r="F4">
+        <v>0.001187054399787047</v>
+      </c>
+      <c r="G4">
+        <v>0.04916595721992851</v>
+      </c>
+      <c r="H4">
+        <v>0.9508340427800716</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>0.06563651825795751</v>
+      </c>
+      <c r="D5">
+        <v>0.0009381491908562051</v>
+      </c>
+      <c r="E5">
+        <v>0.004017276000219924</v>
+      </c>
+      <c r="F5">
+        <v>-0.003079126809363722</v>
+      </c>
+      <c r="G5">
+        <v>0.5661003339318083</v>
+      </c>
+      <c r="H5">
+        <v>0.4338996660681918</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>0.06657466744881371</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0.2179061588686753</v>
+      </c>
+      <c r="D7">
+        <v>-0.1513314914198616</v>
+      </c>
+      <c r="E7">
+        <v>-0.07677906293842739</v>
+      </c>
+      <c r="F7">
+        <v>-0.07455242848143416</v>
+      </c>
+      <c r="G7">
+        <v>0.5073568113156817</v>
+      </c>
+      <c r="H7">
+        <v>0.4926431886843184</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B8">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C8">
         <v>0.2250579911111283</v>
       </c>
-      <c r="D4">
-        <v>-0.1585199366569516</v>
-      </c>
-      <c r="E4">
-        <v>-0.08886230598376316</v>
-      </c>
-      <c r="F4">
-        <v>-0.06965763067318842</v>
-      </c>
-      <c r="G4">
-        <v>0.5605749526387177</v>
-      </c>
-      <c r="H4">
-        <v>0.4394250473612823</v>
+      <c r="D8">
+        <v>-0.1584833236623146</v>
+      </c>
+      <c r="E8">
+        <v>-0.08887279934180774</v>
+      </c>
+      <c r="F8">
+        <v>-0.06961052432050688</v>
+      </c>
+      <c r="G8">
+        <v>0.5607706684090738</v>
+      </c>
+      <c r="H8">
+        <v>0.4392293315909263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>